<commit_message>
Changes per January 6th (LacI model 2 circuits)
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master_Thesis/LacI/code/model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56860A4-4560-D742-AB65-5A08404FD832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FF545E-C797-4F48-A3D1-EABD0E8F23DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41620" yWindow="500" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>names</t>
   </si>
@@ -54,9 +65,6 @@
     <t>kL</t>
   </si>
   <si>
-    <t>atcAdded</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -66,24 +74,15 @@
     <t>plot_names</t>
   </si>
   <si>
-    <t>k_{TetR}</t>
-  </si>
-  <si>
     <t>k_{Cit}</t>
   </si>
   <si>
     <t>d_{Cit}</t>
   </si>
   <si>
-    <t>theta_{TetR}</t>
-  </si>
-  <si>
     <t>ind-time</t>
   </si>
   <si>
-    <t>d_{TetR}</t>
-  </si>
-  <si>
     <t>dCit</t>
   </si>
   <si>
@@ -121,6 +120,24 @@
   </si>
   <si>
     <t>P4Lacn_cit</t>
+  </si>
+  <si>
+    <t>k_{LacI}</t>
+  </si>
+  <si>
+    <t>d_{LacI}</t>
+  </si>
+  <si>
+    <t>theta_{LacI}</t>
+  </si>
+  <si>
+    <t>IPTGAdded</t>
+  </si>
+  <si>
+    <t>LacI_rep_Cit_W220F</t>
+  </si>
+  <si>
+    <t>theta_{LacI_W220F}</t>
   </si>
 </sst>
 </file>
@@ -488,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,12 +533,12 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>0.01</v>
@@ -538,13 +555,13 @@
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1">
         <v>0.01</v>
@@ -562,12 +579,12 @@
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1">
         <v>1E-3</v>
@@ -584,13 +601,13 @@
       <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
+      <c r="G4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>7.0000000000000001E-3</v>
@@ -605,21 +622,22 @@
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5.0000000000000004E-6</v>
+        <v>21</v>
+      </c>
+      <c r="B6" s="2">
+        <f>0.000005*1000</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -631,12 +649,12 @@
         <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -659,7 +677,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
         <v>1.0000000000000001E-5</v>
@@ -682,7 +700,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>1E-3</v>
@@ -699,132 +717,147 @@
       <c r="F9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>16</v>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="C10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
         <v>250</v>
       </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
         <v>250</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="G11" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
         <v>5000</v>
       </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
         <v>5000</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="C13" s="2">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C14" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>1.7299999999999999E-2</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -842,13 +875,13 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
@@ -866,6 +899,14 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes per January 10th (LacI model 3 circuits)
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FF545E-C797-4F48-A3D1-EABD0E8F23DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CD9CEE-3C2F-9548-BA26-9A5A8B6DC235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8600" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>names</t>
   </si>
@@ -138,6 +138,24 @@
   </si>
   <si>
     <t>theta_{LacI_W220F}</t>
+  </si>
+  <si>
+    <t>P_4Lacn_LacI</t>
+  </si>
+  <si>
+    <t>k_{LacI_W220F_Q60G_T167A}</t>
+  </si>
+  <si>
+    <t>P_4Lacn_LacI_L</t>
+  </si>
+  <si>
+    <t>kL_W220F_Q60G_T167A</t>
+  </si>
+  <si>
+    <t>LacI_rep</t>
+  </si>
+  <si>
+    <t>theta_{LacI_W220F_Q60G_T167A}</t>
   </si>
 </sst>
 </file>
@@ -508,7 +526,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,10 +605,10 @@
         <v>26</v>
       </c>
       <c r="B4" s="1">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="C4" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -610,10 +628,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="C5" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -621,8 +639,8 @@
       <c r="E5" s="1">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>13</v>
@@ -703,7 +721,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="1">
-        <v>1E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C9" s="1">
         <v>100</v>
@@ -726,7 +744,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="1">
-        <v>1E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C10" s="1">
         <v>1000</v>
@@ -860,30 +878,75 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C16" s="1">
+        <v>100</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>98</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>100</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -891,7 +954,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -899,7 +962,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Changes per January 10th second push (LacI model 3 circuits)
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CD9CEE-3C2F-9548-BA26-9A5A8B6DC235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD44A7CF-3C6E-DE44-B3BD-7A1070722735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,8 +651,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="2">
-        <f>0.000005*1000</f>
-        <v>5.0000000000000001E-3</v>
+        <v>100</v>
       </c>
       <c r="C6" s="1">
         <v>1000</v>

</xml_diff>

<commit_message>
Changes per January 11th (LacI model 3 working circuits)
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD44A7CF-3C6E-DE44-B3BD-7A1070722735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F5F72D-7075-4D4B-8409-259E36BB4F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,7 +526,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,7 +651,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="2">
-        <v>100</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C6" s="1">
         <v>1000</v>

</xml_diff>

<commit_message>
Changes per January 16th (LacI model 3 working circuits)
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F5F72D-7075-4D4B-8409-259E36BB4F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1192640D-295B-8F4A-95F1-F27BD786C02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15680" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>names</t>
   </si>
@@ -156,6 +156,30 @@
   </si>
   <si>
     <t>theta_{LacI_W220F_Q60G_T167A}</t>
+  </si>
+  <si>
+    <t>Silence_LacI_rep</t>
+  </si>
+  <si>
+    <t>silence</t>
+  </si>
+  <si>
+    <t>pt7_LacI</t>
+  </si>
+  <si>
+    <t>P3_Lacn_5_cit</t>
+  </si>
+  <si>
+    <t>P3_Lacn_5_cit_L</t>
+  </si>
+  <si>
+    <t>k_{pt7_PacI}</t>
+  </si>
+  <si>
+    <t>k_{Cit_Lacn3}</t>
+  </si>
+  <si>
+    <t>kL_cit_pt7</t>
   </si>
 </sst>
 </file>
@@ -526,7 +550,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -945,21 +969,97 @@
         <v>39</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C20" s="2">
+        <v>100</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>98</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="A21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C21" s="1">
+        <v>100</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>92</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>

</xml_diff>

<commit_message>
Changes per January 17th (LacI model 4 circuits)
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1192640D-295B-8F4A-95F1-F27BD786C02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D32C161-65B3-0B44-A133-1B1A60A1C2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15680" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>names</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>kL_cit_pt7</t>
+  </si>
+  <si>
+    <t>dLacI_pt7</t>
+  </si>
+  <si>
+    <t>d_{LacI_pt7}</t>
+  </si>
+  <si>
+    <t>nLacI_P3</t>
+  </si>
+  <si>
+    <t>n_P3</t>
   </si>
 </sst>
 </file>
@@ -547,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,12 +1074,50 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes per January 20th (LacI model 4 circuits)
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D32C161-65B3-0B44-A133-1B1A60A1C2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F421838D-6646-5D41-ACC0-9508764D2018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,11 +561,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -641,10 +644,10 @@
         <v>26</v>
       </c>
       <c r="B4" s="1">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -664,10 +667,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -684,39 +687,39 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>23</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1E-3</v>
       </c>
       <c r="C6" s="1">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>0.9</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -724,45 +727,45 @@
       <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>7</v>
+      <c r="G7" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>21</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.01</v>
       </c>
       <c r="C8" s="1">
-        <v>0.01</v>
+        <v>100</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0.9</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -770,146 +773,146 @@
       <c r="F9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>30</v>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>250</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>250</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>31</v>
+      <c r="G11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>5000</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>5000</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>14</v>
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>100</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>7.7000000000000002E-3</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C13" s="1">
+        <v>100</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>250</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>250</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="C14" s="2">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
+      <c r="G14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>1.7299999999999999E-2</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G15" t="s">
-        <v>19</v>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -940,10 +943,10 @@
         <v>36</v>
       </c>
       <c r="B17" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="C17" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -963,7 +966,7 @@
         <v>38</v>
       </c>
       <c r="B18" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>0.01</v>
       </c>
       <c r="C18" s="1">
         <v>100</v>
@@ -1009,7 +1012,7 @@
         <v>42</v>
       </c>
       <c r="B20" s="2">
-        <v>1.0000000000000001E-5</v>
+        <v>0.01</v>
       </c>
       <c r="C20" s="2">
         <v>100</v>
@@ -1032,7 +1035,7 @@
         <v>43</v>
       </c>
       <c r="B21" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>0.01</v>
       </c>
       <c r="C21" s="1">
         <v>100</v>
@@ -1055,10 +1058,10 @@
         <v>44</v>
       </c>
       <c r="B22" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="C22" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1078,7 +1081,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="1">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -1104,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D24" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Changes per January 23th (LacI model 4 circuits)
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F421838D-6646-5D41-ACC0-9508764D2018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583F99E4-1F39-584B-B27D-186B31B259E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34820" yWindow="680" windowWidth="20140" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>names</t>
   </si>
@@ -62,9 +62,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>kL</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -107,12 +104,6 @@
     <t>nLacI</t>
   </si>
   <si>
-    <t>PAct1_LacI_L</t>
-  </si>
-  <si>
-    <t>LacI_rep_Cit</t>
-  </si>
-  <si>
     <t>IPTG</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
     <t>IPTGAdded</t>
   </si>
   <si>
-    <t>LacI_rep_Cit_W220F</t>
-  </si>
-  <si>
     <t>theta_{LacI_W220F}</t>
   </si>
   <si>
@@ -152,9 +140,6 @@
     <t>kL_W220F_Q60G_T167A</t>
   </si>
   <si>
-    <t>LacI_rep</t>
-  </si>
-  <si>
     <t>theta_{LacI_W220F_Q60G_T167A}</t>
   </si>
   <si>
@@ -192,6 +177,15 @@
   </si>
   <si>
     <t>n_P3</t>
+  </si>
+  <si>
+    <t>LacI_rep_WT</t>
+  </si>
+  <si>
+    <t>LacI_rep_W220F</t>
+  </si>
+  <si>
+    <t>LacI_rep_3mut</t>
   </si>
 </sst>
 </file>
@@ -559,15 +553,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -590,18 +585,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
         <v>0.01</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
+        <f>B2*1000</f>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -613,18 +609,19 @@
         <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>0.01</v>
       </c>
       <c r="C3" s="1">
-        <v>100</v>
+        <f t="shared" ref="C3:C23" si="0">B3*1000</f>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -636,18 +633,19 @@
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="C4" s="1">
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -659,18 +657,19 @@
         <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="C5" s="1">
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -682,444 +681,436 @@
         <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.1</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>8</v>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2">
         <v>0.01</v>
       </c>
       <c r="C7" s="1">
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>30</v>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.01</v>
+      <c r="B8" s="1">
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
+      <c r="A10" t="s">
+        <v>18</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>7.7000000000000002E-3</v>
+        <v>1.7299999999999999E-2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1.7299999999999999E-2</v>
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C12" s="2">
-        <v>100</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G12" t="s">
-        <v>18</v>
+      <c r="G12" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>250</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1">
         <v>0.01</v>
       </c>
-      <c r="C13" s="1">
-        <v>100</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>250</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>250</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>98</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>5000</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>5000</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="C16" s="1">
-        <v>100</v>
-      </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>98</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>37</v>
+      <c r="G17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.01</v>
+        <v>35</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
       </c>
       <c r="C18" s="1">
-        <v>100</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>98</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
         <v>40</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="2">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1">
         <v>0.01</v>
       </c>
-      <c r="C20" s="2">
-        <v>100</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <v>98</v>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>92</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="C21" s="1">
-        <v>100</v>
-      </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>92</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.01</v>
+        <v>45</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.6</v>
+        <v>10</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2">
-        <v>10</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LacImodel 5 circuits, narrowed down parameter boundaries after manual parameter estimation
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583F99E4-1F39-584B-B27D-186B31B259E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB145A2-849E-FC49-A058-EE891E098A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34820" yWindow="680" windowWidth="20140" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19820" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,11 +593,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="1">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="1">
-        <f>B2*1000</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -617,11 +616,10 @@
         <v>24</v>
       </c>
       <c r="B3" s="1">
-        <v>0.01</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C23" si="0">B3*1000</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -641,11 +639,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="1">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -665,11 +662,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -689,11 +685,10 @@
         <v>47</v>
       </c>
       <c r="B6" s="1">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -713,11 +708,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="2">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -740,7 +734,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -763,7 +757,6 @@
         <v>0</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D9" s="2">
@@ -787,7 +780,6 @@
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D10" s="2">
@@ -808,10 +800,9 @@
         <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="D11" s="2">
@@ -835,8 +826,7 @@
         <v>1E-3</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -859,7 +849,6 @@
         <v>0</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D13" s="1">
@@ -883,7 +872,6 @@
         <v>0</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D14" s="1">
@@ -904,10 +892,9 @@
         <v>30</v>
       </c>
       <c r="B15" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D15" s="1">
@@ -931,7 +918,6 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="D16" s="1">
@@ -952,11 +938,10 @@
         <v>49</v>
       </c>
       <c r="B17" s="1">
-        <v>0.01</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1E-3</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -999,10 +984,9 @@
         <v>37</v>
       </c>
       <c r="B19" s="2">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D19" s="2">
@@ -1023,11 +1007,10 @@
         <v>38</v>
       </c>
       <c r="B20" s="1">
-        <v>0.01</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1047,10 +1030,9 @@
         <v>39</v>
       </c>
       <c r="B21" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="D21" s="1">
@@ -1071,10 +1053,9 @@
         <v>43</v>
       </c>
       <c r="B22" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D22" s="1">
@@ -1098,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
LacImodel 5 circuits, 15 starting points, parallel computing
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB145A2-849E-FC49-A058-EE891E098A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4500CC2D-57EC-8246-AAC9-E6C03E827183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19820" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5240" yWindow="800" windowWidth="19820" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>names</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>LacI_rep_3mut</t>
+  </si>
+  <si>
+    <t>theta_{LacI_W220F_Q60G_T167A-pt7}</t>
+  </si>
+  <si>
+    <t>LacI_rep_3mut_P3</t>
   </si>
 </sst>
 </file>
@@ -553,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,7 +602,7 @@
         <v>0.1</v>
       </c>
       <c r="C2" s="1">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -616,10 +622,10 @@
         <v>24</v>
       </c>
       <c r="B3" s="1">
-        <v>15</v>
+        <v>0.1</v>
       </c>
       <c r="C3" s="1">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -639,7 +645,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="1">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C4" s="1">
         <v>0.1</v>
@@ -662,7 +668,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C5" s="1">
         <v>0.1</v>
@@ -688,7 +694,7 @@
         <v>0.01</v>
       </c>
       <c r="C6" s="1">
-        <v>0.05</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -731,10 +737,10 @@
         <v>21</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -826,7 +832,7 @@
         <v>1E-3</v>
       </c>
       <c r="C12" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -892,10 +898,10 @@
         <v>30</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C15" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -941,7 +947,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C17" s="1">
-        <v>1E-3</v>
+        <v>0.1</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -984,10 +990,10 @@
         <v>37</v>
       </c>
       <c r="B19" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C19" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -1007,10 +1013,10 @@
         <v>38</v>
       </c>
       <c r="B20" s="1">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="C20" s="1">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1030,7 +1036,7 @@
         <v>39</v>
       </c>
       <c r="B21" s="1">
-        <v>1E-3</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C21" s="1">
         <v>0.01</v>
@@ -1053,7 +1059,7 @@
         <v>43</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="C22" s="1">
         <v>10</v>
@@ -1076,10 +1082,10 @@
         <v>45</v>
       </c>
       <c r="B23" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C23" s="1">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -1092,6 +1098,29 @@
       </c>
       <c r="G23" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes: readdataLacIm.m -> no longer saved as data_mutations. data.time no longer 20 minutes but 1200 minutes. Search of correct data according to strain. Simulation functions: Data is no longer opened in simulation function (already in objective function). Model: Changes of model equation according to progress report (Leakage term not in nominator & Leakage + production * repression - degradation)
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4500CC2D-57EC-8246-AAC9-E6C03E827183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD065229-195B-0F4A-8C00-C05AA44CC56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="800" windowWidth="19820" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33700" yWindow="500" windowWidth="35180" windowHeight="25320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,7 +671,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C5" s="1">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -691,7 +691,7 @@
         <v>47</v>
       </c>
       <c r="B6" s="1">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="C6" s="1">
         <v>10</v>
@@ -714,7 +714,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C7" s="1">
         <v>100</v>
@@ -740,7 +740,7 @@
         <v>0.5</v>
       </c>
       <c r="C8" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -829,7 +829,7 @@
         <v>48</v>
       </c>
       <c r="B12" s="1">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -990,10 +990,10 @@
         <v>37</v>
       </c>
       <c r="B19" s="2">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C19" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -1059,10 +1059,10 @@
         <v>43</v>
       </c>
       <c r="B22" s="1">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="C22" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Changes: changed model euqations back
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD065229-195B-0F4A-8C00-C05AA44CC56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8B2F89-D29A-784F-8509-30D310767AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33700" yWindow="500" windowWidth="35180" windowHeight="25320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,7 +562,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,10 +599,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -645,10 +645,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C4" s="1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -714,10 +714,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="2">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C7" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -829,10 +829,10 @@
         <v>48</v>
       </c>
       <c r="B12" s="1">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -921,10 +921,10 @@
         <v>32</v>
       </c>
       <c r="B16" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C16" s="1">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -944,10 +944,10 @@
         <v>49</v>
       </c>
       <c r="B17" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C17" s="1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -990,10 +990,10 @@
         <v>37</v>
       </c>
       <c r="B19" s="2">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="C19" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -1036,10 +1036,10 @@
         <v>39</v>
       </c>
       <c r="B21" s="1">
-        <v>9.9999999999999995E-7</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="C21" s="1">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1059,10 +1059,10 @@
         <v>43</v>
       </c>
       <c r="B22" s="1">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1105,10 +1105,10 @@
         <v>51</v>
       </c>
       <c r="B24" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C24" s="1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Changes: second part of project -> uncertainty analysis
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8B2F89-D29A-784F-8509-30D310767AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C014E8-19C0-7C42-BF41-C40E018A808B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -562,7 +562,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -680,7 +680,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -815,10 +815,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
+        <v>12.2533526453471</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Changes: second part of project -> uncertainty analysis; simulation of random parameter draws
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C014E8-19C0-7C42-BF41-C40E018A808B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755AC829-718A-694D-B769-A7986270874E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -562,7 +562,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -818,7 +818,7 @@
         <v>12.2533526453471</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Changes: EC50, EC90, EC10, slope calculations from simulation using parameters drawn from hyperspace, from PESTO and from PESTO CI
</commit_message>
<xml_diff>
--- a/Master_Thesis/LacI/code/model/parameters_0.xlsx
+++ b/Master_Thesis/LacI/code/model/parameters_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiobroger/Documents/ETH/Master/Master_Thesis/LacI/code/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755AC829-718A-694D-B769-A7986270874E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF5EBBA-C014-2D40-BA23-BB5F29FB4B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -562,7 +562,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>